<commit_message>
Comentando e apagando códigos inúteis
</commit_message>
<xml_diff>
--- a/planilhas/automacoestemp.xlsx
+++ b/planilhas/automacoestemp.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,7 +432,29 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modifições nos metodos da classe planilha
</commit_message>
<xml_diff>
--- a/planilhas/automacoestemp.xlsx
+++ b/planilhas/automacoestemp.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,29 +432,7 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Lâmpada</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D1" t="b">
-        <v>0</v>
-      </c>
-      <c r="F1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mudança no botão de ativar automação
</commit_message>
<xml_diff>
--- a/planilhas/automacoestemp.xlsx
+++ b/planilhas/automacoestemp.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,7 +432,74 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>l2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>tv</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicionada mensagem na confirmação das automações
</commit_message>
<xml_diff>
--- a/planilhas/automacoestemp.xlsx
+++ b/planilhas/automacoestemp.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,7 +432,74 @@
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="2" min="4" max="4"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ar</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>tv</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>lamp1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mudança nas cores do botões
</commit_message>
<xml_diff>
--- a/planilhas/automacoestemp.xlsx
+++ b/planilhas/automacoestemp.xlsx
@@ -475,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -496,7 +496,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>